<commit_message>
restructured the flask application and added the connection the the maria database.
</commit_message>
<xml_diff>
--- a/pokemon_data.xlsx
+++ b/pokemon_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy Dixon\Documents\UMBC\2020\Summer\CMSC491\Weekly_Assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\python_projects\cmsc433\final_project\cmsc433-pokemon-game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62EDDD70-60FA-4625-B193-76C378453853}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8429E0D2-2F98-4D1E-9965-84743D9B6797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-28920" yWindow="-1575" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pokemon" sheetId="1" r:id="rId1"/>
@@ -2518,7 +2518,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3057,9 +3057,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3097,7 +3097,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3203,7 +3203,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3345,17 +3345,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M801"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>